<commit_message>
conf. vendors for test purposes
</commit_message>
<xml_diff>
--- a/vendors.xlsx
+++ b/vendors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I1000928\Projects\smart-document-renamer\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I1000928\Projects\smart-document-renamer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD86ADBA-4304-465A-844C-05AD8316161A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF1270F-5C01-4EB4-B80E-57195EC905A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{F34DF576-2CC0-49DE-B50B-71A003A2F59E}"/>
+    <workbookView xWindow="14535" yWindow="-16395" windowWidth="29040" windowHeight="15720" xr2:uid="{F34DF576-2CC0-49DE-B50B-71A003A2F59E}"/>
   </bookViews>
   <sheets>
     <sheet name="test_spreadsheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="236">
   <si>
     <t>#</t>
   </si>
@@ -37,21 +37,9 @@
 3</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
-    <t>House Music Limited</t>
-  </si>
-  <si>
-    <t>Music Lover</t>
-  </si>
-  <si>
-    <t>Orange Rower</t>
-  </si>
-  <si>
     <t>Owner</t>
   </si>
   <si>
@@ -61,10 +49,835 @@
     <t>Vendor</t>
   </si>
   <si>
-    <t>Starboard Or Port Inc</t>
-  </si>
-  <si>
-    <t>ABC &amp; DEF Inc</t>
+    <t xml:space="preserve">	'
+0005'</t>
+  </si>
+  <si>
+    <t>Abby Rating Systems</t>
+  </si>
+  <si>
+    <t>Brandii Mitchell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2268'</t>
+  </si>
+  <si>
+    <t>Above IT, LLC</t>
+  </si>
+  <si>
+    <t>Towanda Morales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0032'</t>
+  </si>
+  <si>
+    <t>Agency Computer Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7215'</t>
+  </si>
+  <si>
+    <t>Boon Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1764'</t>
+  </si>
+  <si>
+    <t>Boston Software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2010'</t>
+  </si>
+  <si>
+    <t>Carrier &amp;amp; Technology Solutions-InsurePay</t>
+  </si>
+  <si>
+    <t>Syed Zaki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4770'</t>
+  </si>
+  <si>
+    <t>CCI Computer Services, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4248'</t>
+  </si>
+  <si>
+    <t>CGI Technologies and Solutions, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1749'</t>
+  </si>
+  <si>
+    <t>ClarionDoor</t>
+  </si>
+  <si>
+    <t>Ciaran O'Connor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6363'</t>
+  </si>
+  <si>
+    <t>Computer Sciences Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6804'</t>
+  </si>
+  <si>
+    <t>CRAWFORD AND COMPANY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2088'</t>
+  </si>
+  <si>
+    <t>DF Institute d.b.a. Kaplan Financial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2050'</t>
+  </si>
+  <si>
+    <t>Duck Creek Technologies LLC</t>
+  </si>
+  <si>
+    <t>Kiara Keaton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+3948'</t>
+  </si>
+  <si>
+    <t>Dyad, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2334'</t>
+  </si>
+  <si>
+    <t>Earnix, Inc</t>
+  </si>
+  <si>
+    <t>Dannon Thompson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1878'</t>
+  </si>
+  <si>
+    <t>eBaoTech International Pte. LTD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0009'</t>
+  </si>
+  <si>
+    <t>EXAMFX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2011'</t>
+  </si>
+  <si>
+    <t>Federato Technologies, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2265'</t>
+  </si>
+  <si>
+    <t>FilingRamp LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+3238'</t>
+  </si>
+  <si>
+    <t>GhostDraft /CCM Enterprises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4256'</t>
+  </si>
+  <si>
+    <t>Guidewire InsuranceNow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4575'</t>
+  </si>
+  <si>
+    <t>GUIDEWIRE SOFTWARE, INC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4005'</t>
+  </si>
+  <si>
+    <t>IMT Computer Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4020'</t>
+  </si>
+  <si>
+    <t>InformINS, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1054'</t>
+  </si>
+  <si>
+    <t>Innovative Computer Systems, Inc. d/b/a Finys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4079'</t>
+  </si>
+  <si>
+    <t>Instanda - F
+2X Group Limited</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0822'</t>
+  </si>
+  <si>
+    <t>INSTEC Insurance Information Technologies, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7002'</t>
+  </si>
+  <si>
+    <t>Insurance Data Processing, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4098'</t>
+  </si>
+  <si>
+    <t>Insurance Technologies Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4097'</t>
+  </si>
+  <si>
+    <t>Insurance Technology Solutions, LLC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4203'</t>
+  </si>
+  <si>
+    <t>Insuresoft LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6382'</t>
+  </si>
+  <si>
+    <t>Insurity, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4158'</t>
+  </si>
+  <si>
+    <t>International Risk Management Institute, Inc. (IRMI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4187'</t>
+  </si>
+  <si>
+    <t>Intuitive Web Solutions, LLC d.b.a. Britecore LLC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5410'</t>
+  </si>
+  <si>
+    <t>Jetfile Technologies Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0422'</t>
+  </si>
+  <si>
+    <t>LEXIS NEXIS,  A DIVISION OF REED ELSEVIER INC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4109'</t>
+  </si>
+  <si>
+    <t>LexisNexis Risk Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'TBD'</t>
+  </si>
+  <si>
+    <t>Lowry &amp;amp; Associates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2032'</t>
+  </si>
+  <si>
+    <t>Majesco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4727'</t>
+  </si>
+  <si>
+    <t>Martin and Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4622'</t>
+  </si>
+  <si>
+    <t>MFXChange US, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5493'</t>
+  </si>
+  <si>
+    <t>MGA Systems, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0610'</t>
+  </si>
+  <si>
+    <t>Modotech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5510'</t>
+  </si>
+  <si>
+    <t>National Underwriter Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5304'</t>
+  </si>
+  <si>
+    <t>NeST Technologies Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1851'</t>
+  </si>
+  <si>
+    <t>One, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6008'</t>
+  </si>
+  <si>
+    <t>OneShield, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+2223'</t>
+  </si>
+  <si>
+    <t>OneSys Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6009'</t>
+  </si>
+  <si>
+    <t>Origami Risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6214'</t>
+  </si>
+  <si>
+    <t>Perr &amp;amp; Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0727'</t>
+  </si>
+  <si>
+    <t>Property &amp;amp; Casualty Management Systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+9174'</t>
+  </si>
+  <si>
+    <t>Quick Silver Systems, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+3976'</t>
+  </si>
+  <si>
+    <t>QuotePro, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5805'</t>
+  </si>
+  <si>
+    <t>Sapiens Americas Corp. (Maximum Processing Inc).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1052'</t>
+  </si>
+  <si>
+    <t>Sapiens Americas Corporation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8649'</t>
+  </si>
+  <si>
+    <t>Silvervine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1886'</t>
+  </si>
+  <si>
+    <t>Snap-On Diagnostics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7406'</t>
+  </si>
+  <si>
+    <t>Solartis, LLC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6882'</t>
+  </si>
+  <si>
+    <t>SpeedBuilder Systems, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+6367'</t>
+  </si>
+  <si>
+    <t>S&amp;amp;P Global (aka Polk)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7491'</t>
+  </si>
+  <si>
+    <t>STANDARD PUBLISHING CORPORATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7873'</t>
+  </si>
+  <si>
+    <t>Trans World Data, LLC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+7750'</t>
+  </si>
+  <si>
+    <t>Two Sigma Insurance Quantified, LP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+1050'</t>
+  </si>
+  <si>
+    <t>Unisoft Communications, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+4267'</t>
+  </si>
+  <si>
+    <t>United Software Developers, Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8449'</t>
+  </si>
+  <si>
+    <t>ValueMomentum, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0091'</t>
+  </si>
+  <si>
+    <t>Vertafore, Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+0087F'</t>
+  </si>
+  <si>
+    <t>Vertafore Reference Connect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8404'</t>
+  </si>
+  <si>
+    <t>Virtual MGA Ltd. Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8586'</t>
+  </si>
+  <si>
+    <t>WaterStreet Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+5073'</t>
+  </si>
+  <si>
+    <t>West Services Inc fka Thomson Reuters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+9553'</t>
+  </si>
+  <si>
+    <t>Willis Towers Watson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8033'</t>
+  </si>
+  <si>
+    <t>Wolters Kluwer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+8599'</t>
+  </si>
+  <si>
+    <t>Xceedance Consulting Ltd (Xceedance)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	'
+9658'</t>
+  </si>
+  <si>
+    <t>Zywave, Inc.</t>
   </si>
 </sst>
 </file>
@@ -218,7 +1031,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +1219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -584,11 +1403,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -597,6 +1413,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -973,10 +1795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBC3EE0-6EAA-4467-8C9B-5BD58485DF43}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -988,71 +1810,1079 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1234</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>5678</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="5" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>9101</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A62" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A64" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A65" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A69" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A73" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A75" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>